<commit_message>
Änderung Anforderungsanalyse und Zeitplan
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BLJ\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F38A26D-58B9-4283-A40A-95990752C070}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A4C96C-6AF2-4FF6-BEEC-C0EC8930BC0B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="4050" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
   <si>
     <t>Nr.</t>
   </si>
@@ -257,7 +257,7 @@
     <t>Verschiedene Schlangenfarben</t>
   </si>
   <si>
-    <t>M = Meilensteingespräch</t>
+    <t>Mauern zufällig generieren</t>
   </si>
 </sst>
 </file>
@@ -1437,12 +1437,17 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1474,13 +1479,8 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1585,10 +1585,10 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -1597,7 +1597,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1659,10 +1659,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2169,8 +2169,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AQ37" sqref="AQ37:AQ38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AB28" sqref="AB28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2301,29 +2301,11 @@
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="93" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="6"/>
       <c r="AI3" s="6"/>
       <c r="AJ3" s="6"/>
-      <c r="AK3" s="6"/>
+      <c r="AK3" s="92"/>
       <c r="AL3" s="6"/>
       <c r="AM3" s="6"/>
       <c r="AN3" s="6"/>
@@ -2491,88 +2473,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="94"/>
+      <c r="D7" s="95"/>
       <c r="E7" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="95" t="s">
+      <c r="G7" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95"/>
-      <c r="M7" s="96"/>
-      <c r="N7" s="95" t="s">
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="95"/>
-      <c r="P7" s="95"/>
-      <c r="Q7" s="95"/>
-      <c r="R7" s="95"/>
-      <c r="S7" s="95"/>
-      <c r="T7" s="96"/>
-      <c r="U7" s="95" t="s">
+      <c r="O7" s="96"/>
+      <c r="P7" s="96"/>
+      <c r="Q7" s="96"/>
+      <c r="R7" s="96"/>
+      <c r="S7" s="96"/>
+      <c r="T7" s="97"/>
+      <c r="U7" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="V7" s="95"/>
-      <c r="W7" s="95"/>
-      <c r="X7" s="95"/>
-      <c r="Y7" s="95"/>
-      <c r="Z7" s="95"/>
-      <c r="AA7" s="96"/>
-      <c r="AB7" s="97" t="s">
+      <c r="V7" s="96"/>
+      <c r="W7" s="96"/>
+      <c r="X7" s="96"/>
+      <c r="Y7" s="96"/>
+      <c r="Z7" s="96"/>
+      <c r="AA7" s="97"/>
+      <c r="AB7" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="AC7" s="95"/>
-      <c r="AD7" s="95"/>
-      <c r="AE7" s="95"/>
-      <c r="AF7" s="95"/>
-      <c r="AG7" s="95"/>
-      <c r="AH7" s="96"/>
-      <c r="AI7" s="95" t="s">
+      <c r="AC7" s="96"/>
+      <c r="AD7" s="96"/>
+      <c r="AE7" s="96"/>
+      <c r="AF7" s="96"/>
+      <c r="AG7" s="96"/>
+      <c r="AH7" s="97"/>
+      <c r="AI7" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="AJ7" s="95"/>
-      <c r="AK7" s="95"/>
-      <c r="AL7" s="95"/>
-      <c r="AM7" s="95"/>
-      <c r="AN7" s="95"/>
-      <c r="AO7" s="96"/>
-      <c r="AP7" s="97" t="s">
+      <c r="AJ7" s="96"/>
+      <c r="AK7" s="96"/>
+      <c r="AL7" s="96"/>
+      <c r="AM7" s="96"/>
+      <c r="AN7" s="96"/>
+      <c r="AO7" s="97"/>
+      <c r="AP7" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="AQ7" s="95"/>
-      <c r="AR7" s="95"/>
-      <c r="AS7" s="95"/>
-      <c r="AT7" s="95"/>
-      <c r="AU7" s="95"/>
-      <c r="AV7" s="96"/>
-      <c r="AW7" s="95" t="s">
+      <c r="AQ7" s="96"/>
+      <c r="AR7" s="96"/>
+      <c r="AS7" s="96"/>
+      <c r="AT7" s="96"/>
+      <c r="AU7" s="96"/>
+      <c r="AV7" s="97"/>
+      <c r="AW7" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="AX7" s="95"/>
-      <c r="AY7" s="95"/>
-      <c r="AZ7" s="95"/>
-      <c r="BA7" s="95"/>
-      <c r="BB7" s="95"/>
-      <c r="BC7" s="96"/>
-      <c r="BD7" s="97" t="s">
+      <c r="AX7" s="96"/>
+      <c r="AY7" s="96"/>
+      <c r="AZ7" s="96"/>
+      <c r="BA7" s="96"/>
+      <c r="BB7" s="96"/>
+      <c r="BC7" s="97"/>
+      <c r="BD7" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="BE7" s="95"/>
-      <c r="BF7" s="95"/>
-      <c r="BG7" s="95"/>
-      <c r="BH7" s="95"/>
-      <c r="BI7" s="95"/>
-      <c r="BJ7" s="98"/>
+      <c r="BE7" s="96"/>
+      <c r="BF7" s="96"/>
+      <c r="BG7" s="96"/>
+      <c r="BH7" s="96"/>
+      <c r="BI7" s="96"/>
+      <c r="BJ7" s="99"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -3114,8 +3096,7 @@
       <c r="AP13" s="59"/>
       <c r="AQ13" s="60"/>
       <c r="AR13" s="55"/>
-      <c r="AS13" s="87"/>
-      <c r="AT13" s="55"/>
+      <c r="AT13" s="87"/>
       <c r="AU13" s="66"/>
       <c r="AV13" s="67"/>
       <c r="AW13" s="59"/>
@@ -3142,11 +3123,11 @@
       </c>
       <c r="C14" s="41">
         <f>SUM(C15:C17)</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="D14" s="42">
         <f>SUM(D15:D17)</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="31"/>
@@ -3219,7 +3200,7 @@
       </c>
       <c r="D15" s="83">
         <f>SUM(G15:BJ15)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="89" t="s">
@@ -3227,9 +3208,15 @@
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="54"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="63"/>
+      <c r="I15" s="68">
+        <v>4</v>
+      </c>
+      <c r="J15" s="87">
+        <v>1</v>
+      </c>
+      <c r="K15" s="63">
+        <v>1</v>
+      </c>
       <c r="L15" s="57"/>
       <c r="M15" s="58"/>
       <c r="N15" s="53"/>
@@ -3290,11 +3277,11 @@
         <v>28</v>
       </c>
       <c r="C16" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="83">
         <f>SUM(G16:BJ16)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E16" s="50"/>
       <c r="F16" s="51"/>
@@ -3302,7 +3289,9 @@
       <c r="H16" s="60"/>
       <c r="I16" s="55"/>
       <c r="J16" s="55"/>
-      <c r="K16" s="63"/>
+      <c r="K16" s="63">
+        <v>1.5</v>
+      </c>
       <c r="L16" s="57"/>
       <c r="M16" s="58"/>
       <c r="N16" s="59"/>
@@ -3433,11 +3422,11 @@
       </c>
       <c r="C18" s="41">
         <f>SUM(C19:C30)</f>
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3506,7 +3495,7 @@
         <v>34</v>
       </c>
       <c r="C19" s="49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D19" s="83">
         <f>SUM(G19:BJ19)</f>
@@ -3579,32 +3568,41 @@
         <v>48</v>
       </c>
       <c r="C20" s="49">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="51"/>
       <c r="G20" s="59"/>
       <c r="H20" s="60"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="56"/>
+      <c r="I20" s="68">
+        <v>4</v>
+      </c>
+      <c r="J20" s="68">
+        <v>6</v>
+      </c>
+      <c r="K20" s="68">
+        <v>2</v>
+      </c>
       <c r="L20" s="57"/>
       <c r="M20" s="58"/>
       <c r="N20" s="59"/>
       <c r="O20" s="60"/>
-      <c r="P20" s="55"/>
-      <c r="Q20" s="55"/>
-      <c r="R20" s="56"/>
+      <c r="P20" s="68">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="68"/>
+      <c r="R20" s="68"/>
       <c r="S20" s="57"/>
       <c r="T20" s="58"/>
       <c r="U20" s="59"/>
       <c r="V20" s="60"/>
-      <c r="W20" s="55"/>
-      <c r="X20" s="55"/>
-      <c r="Y20" s="56"/>
+      <c r="W20" s="68"/>
+      <c r="X20" s="68"/>
+      <c r="Y20" s="68"/>
       <c r="Z20" s="57"/>
       <c r="AA20" s="58"/>
       <c r="AB20" s="59"/>
@@ -3623,9 +3621,8 @@
       <c r="AO20" s="58"/>
       <c r="AP20" s="59"/>
       <c r="AQ20" s="60"/>
-      <c r="AR20" s="55"/>
-      <c r="AS20" s="55"/>
-      <c r="AT20" s="56"/>
+      <c r="AR20" s="68"/>
+      <c r="AT20" s="55"/>
       <c r="AU20" s="57"/>
       <c r="AV20" s="58"/>
       <c r="AW20" s="59"/>
@@ -3651,11 +3648,11 @@
         <v>50</v>
       </c>
       <c r="C21" s="49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D21" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E21" s="50"/>
       <c r="F21" s="52"/>
@@ -3663,7 +3660,9 @@
       <c r="H21" s="60"/>
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
-      <c r="K21" s="63"/>
+      <c r="K21" s="63">
+        <v>3</v>
+      </c>
       <c r="L21" s="57"/>
       <c r="M21" s="58"/>
       <c r="N21" s="59"/>
@@ -3724,7 +3723,7 @@
         <v>51</v>
       </c>
       <c r="C22" s="91">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
@@ -3797,7 +3796,7 @@
         <v>52</v>
       </c>
       <c r="C23" s="49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
@@ -3815,7 +3814,6 @@
       <c r="N23" s="59"/>
       <c r="O23" s="60"/>
       <c r="P23" s="61"/>
-      <c r="Q23" s="61"/>
       <c r="R23" s="90"/>
       <c r="S23" s="57"/>
       <c r="T23" s="58"/>
@@ -3869,7 +3867,7 @@
         <v>58</v>
       </c>
       <c r="C24" s="49">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D24" s="83">
         <f t="shared" si="0"/>
@@ -3941,7 +3939,7 @@
         <v>54</v>
       </c>
       <c r="C25" s="49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" s="83">
         <f t="shared" si="0"/>
@@ -3960,7 +3958,7 @@
       <c r="O25" s="60"/>
       <c r="P25" s="55"/>
       <c r="Q25" s="55"/>
-      <c r="R25" s="103"/>
+      <c r="R25" s="93"/>
       <c r="S25" s="57"/>
       <c r="T25" s="58"/>
       <c r="U25" s="59"/>
@@ -4010,7 +4008,7 @@
         <v>55</v>
       </c>
       <c r="C26" s="49">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D26" s="83">
         <f t="shared" si="0"/>
@@ -4034,10 +4032,9 @@
       <c r="T26" s="58"/>
       <c r="U26" s="59"/>
       <c r="V26" s="60"/>
-      <c r="W26" s="104"/>
-      <c r="Y26" s="92" t="s">
-        <v>16</v>
-      </c>
+      <c r="W26" s="94"/>
+      <c r="X26" s="90"/>
+      <c r="Y26" s="104"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
       <c r="AB26" s="59"/>
@@ -4084,7 +4081,7 @@
         <v>56</v>
       </c>
       <c r="C27" s="49">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D27" s="83">
         <f t="shared" si="0"/>
@@ -4181,8 +4178,7 @@
       <c r="U28" s="59"/>
       <c r="V28" s="60"/>
       <c r="W28" s="55"/>
-      <c r="X28" s="68"/>
-      <c r="Y28" s="56"/>
+      <c r="Y28" s="68"/>
       <c r="Z28" s="57"/>
       <c r="AA28" s="58"/>
       <c r="AB28" s="59"/>
@@ -4229,7 +4225,7 @@
         <v>57</v>
       </c>
       <c r="C29" s="49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="83">
         <f t="shared" si="0"/>
@@ -4298,8 +4294,12 @@
       <c r="A30" s="12">
         <v>312</v>
       </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="49"/>
+      <c r="B30" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="49">
+        <v>8</v>
+      </c>
       <c r="D30" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4343,7 +4343,7 @@
       <c r="AO30" s="58"/>
       <c r="AP30" s="69"/>
       <c r="AQ30" s="70"/>
-      <c r="AR30" s="55"/>
+      <c r="AR30" s="68"/>
       <c r="AS30" s="55"/>
       <c r="AT30" s="56"/>
       <c r="AU30" s="57"/>
@@ -4949,7 +4949,7 @@
       </c>
       <c r="C39" s="41">
         <f>SUM(C40:C42)</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="D39" s="42">
         <f>SUM(D40:D42)</f>
@@ -5067,8 +5067,8 @@
       <c r="AO40" s="58"/>
       <c r="AP40" s="53"/>
       <c r="AQ40" s="54"/>
-      <c r="AR40" s="68"/>
-      <c r="AS40" s="55"/>
+      <c r="AR40" s="55"/>
+      <c r="AS40" s="68"/>
       <c r="AT40" s="56"/>
       <c r="AU40" s="57"/>
       <c r="AV40" s="58"/>
@@ -5095,7 +5095,7 @@
         <v>31</v>
       </c>
       <c r="C41" s="49">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="D41" s="83">
         <f t="shared" ref="D41:D42" si="2">SUM(G41:BJ41)</f>
@@ -5140,8 +5140,8 @@
       <c r="AO41" s="58"/>
       <c r="AP41" s="59"/>
       <c r="AQ41" s="60"/>
-      <c r="AR41" s="68"/>
-      <c r="AS41" s="55"/>
+      <c r="AR41" s="55"/>
+      <c r="AS41" s="68"/>
       <c r="AT41" s="56"/>
       <c r="AU41" s="57"/>
       <c r="AV41" s="58"/>
@@ -5236,11 +5236,11 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>38</v>
+        <v>80.5</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>0</v>
+        <v>25.5</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5254,15 +5254,15 @@
       </c>
       <c r="I43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="L43" s="39">
         <f t="shared" si="3"/>
@@ -5282,7 +5282,7 @@
       </c>
       <c r="P43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
@@ -5515,10 +5515,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.4" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="102"/>
+      <c r="B2" s="103"/>
       <c r="C2" s="79" t="s">
         <v>14</v>
       </c>
@@ -5527,11 +5527,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="99" t="str">
+      <c r="A3" s="100" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="100"/>
+      <c r="B3" s="101"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
         <v>6</v>
@@ -5544,45 +5544,45 @@
       <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="99" t="str">
+      <c r="A4" s="100" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="100"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="D4" s="80">
         <f>Zeitplanung!D14</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="E4" s="82"/>
       <c r="F4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="99" t="str">
+      <c r="A5" s="100" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="100"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="99" t="str">
+      <c r="A6" s="100" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="80">
         <f>Zeitplanung!C31</f>
         <v>1</v>
@@ -5594,11 +5594,11 @@
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="99" t="str">
+      <c r="A7" s="100" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="100"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
         <v>1</v>
@@ -5610,14 +5610,14 @@
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="99" t="str">
+      <c r="A8" s="100" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="100"/>
+      <c r="B8" s="101"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="D8" s="80">
         <f>Zeitplanung!D39</f>

</xml_diff>

<commit_message>
schlange bewegen + äpfelfunktionen. bewegen funktioniert noch nicht
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BLJ\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F178D961-5E55-40FA-A9A6-CD0C2543FFE5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE473A8-178B-4882-9A1E-AF3631F6560F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="4050" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1662,7 +1662,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2169,8 +2169,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="96" zoomScaleNormal="96" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3426,7 +3426,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3572,7 +3572,7 @@
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="51"/>
@@ -3594,7 +3594,9 @@
       <c r="P20" s="68">
         <v>3</v>
       </c>
-      <c r="Q20" s="68"/>
+      <c r="Q20" s="68">
+        <v>2</v>
+      </c>
       <c r="R20" s="68"/>
       <c r="S20" s="57"/>
       <c r="T20" s="58"/>
@@ -3727,7 +3729,7 @@
       </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E22" s="50"/>
       <c r="F22" s="51"/>
@@ -3743,7 +3745,9 @@
       <c r="P22" s="68">
         <v>5</v>
       </c>
-      <c r="Q22" s="68"/>
+      <c r="Q22" s="68">
+        <v>3</v>
+      </c>
       <c r="R22" s="56"/>
       <c r="S22" s="57"/>
       <c r="T22" s="58"/>
@@ -3802,7 +3806,7 @@
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="50"/>
       <c r="F23" s="51"/>
@@ -3816,6 +3820,9 @@
       <c r="N23" s="59"/>
       <c r="O23" s="60"/>
       <c r="P23" s="61"/>
+      <c r="Q23" s="5">
+        <v>1</v>
+      </c>
       <c r="R23" s="90"/>
       <c r="S23" s="57"/>
       <c r="T23" s="58"/>
@@ -3873,7 +3880,7 @@
       </c>
       <c r="D24" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="50"/>
       <c r="F24" s="51"/>
@@ -3887,7 +3894,9 @@
       <c r="N24" s="59"/>
       <c r="O24" s="60"/>
       <c r="P24" s="55"/>
-      <c r="Q24" s="55"/>
+      <c r="Q24" s="55">
+        <v>1</v>
+      </c>
       <c r="R24" s="90"/>
       <c r="S24" s="57"/>
       <c r="T24" s="58"/>
@@ -3945,7 +3954,7 @@
       </c>
       <c r="D25" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="50"/>
       <c r="F25" s="51"/>
@@ -3959,7 +3968,9 @@
       <c r="N25" s="59"/>
       <c r="O25" s="60"/>
       <c r="P25" s="55"/>
-      <c r="Q25" s="55"/>
+      <c r="Q25" s="55">
+        <v>1</v>
+      </c>
       <c r="R25" s="93"/>
       <c r="S25" s="57"/>
       <c r="T25" s="58"/>
@@ -5242,7 +5253,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>30.5</v>
+        <v>38.5</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5288,7 +5299,7 @@
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R43" s="39">
         <f t="shared" si="3"/>
@@ -5574,7 +5585,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
Zeitplanung aktualisiert und Schlange versucht zu bewegen
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BLJ\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE473A8-178B-4882-9A1E-AF3631F6560F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B0D2B0-232A-4B11-A2C6-6DF79B25556F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="4050" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
   <si>
     <t>Nr.</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Mauern zufällig generieren</t>
+  </si>
+  <si>
+    <t>***</t>
   </si>
 </sst>
 </file>
@@ -267,7 +270,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
@@ -379,13 +382,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF92D050"/>
+      <color theme="1"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -1129,7 +1126,7 @@
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1440,14 +1437,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1481,6 +1470,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1662,7 +1655,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2169,8 +2162,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="96" zoomScaleNormal="96" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="96" zoomScaleNormal="96" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2473,88 +2466,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="96"/>
+      <c r="D7" s="94"/>
       <c r="E7" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="97" t="s">
+      <c r="G7" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="97"/>
-      <c r="I7" s="97"/>
-      <c r="J7" s="97"/>
-      <c r="K7" s="97"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="97" t="s">
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="97"/>
-      <c r="P7" s="97"/>
-      <c r="Q7" s="97"/>
-      <c r="R7" s="97"/>
-      <c r="S7" s="97"/>
-      <c r="T7" s="98"/>
-      <c r="U7" s="97" t="s">
+      <c r="O7" s="95"/>
+      <c r="P7" s="95"/>
+      <c r="Q7" s="95"/>
+      <c r="R7" s="95"/>
+      <c r="S7" s="95"/>
+      <c r="T7" s="96"/>
+      <c r="U7" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="V7" s="97"/>
-      <c r="W7" s="97"/>
-      <c r="X7" s="97"/>
-      <c r="Y7" s="97"/>
-      <c r="Z7" s="97"/>
-      <c r="AA7" s="98"/>
-      <c r="AB7" s="99" t="s">
+      <c r="V7" s="95"/>
+      <c r="W7" s="95"/>
+      <c r="X7" s="95"/>
+      <c r="Y7" s="95"/>
+      <c r="Z7" s="95"/>
+      <c r="AA7" s="96"/>
+      <c r="AB7" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="AC7" s="97"/>
-      <c r="AD7" s="97"/>
-      <c r="AE7" s="97"/>
-      <c r="AF7" s="97"/>
-      <c r="AG7" s="97"/>
-      <c r="AH7" s="98"/>
-      <c r="AI7" s="97" t="s">
+      <c r="AC7" s="95"/>
+      <c r="AD7" s="95"/>
+      <c r="AE7" s="95"/>
+      <c r="AF7" s="95"/>
+      <c r="AG7" s="95"/>
+      <c r="AH7" s="96"/>
+      <c r="AI7" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="AJ7" s="97"/>
-      <c r="AK7" s="97"/>
-      <c r="AL7" s="97"/>
-      <c r="AM7" s="97"/>
-      <c r="AN7" s="97"/>
-      <c r="AO7" s="98"/>
-      <c r="AP7" s="99" t="s">
+      <c r="AJ7" s="95"/>
+      <c r="AK7" s="95"/>
+      <c r="AL7" s="95"/>
+      <c r="AM7" s="95"/>
+      <c r="AN7" s="95"/>
+      <c r="AO7" s="96"/>
+      <c r="AP7" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="AQ7" s="97"/>
-      <c r="AR7" s="97"/>
-      <c r="AS7" s="97"/>
-      <c r="AT7" s="97"/>
-      <c r="AU7" s="97"/>
-      <c r="AV7" s="98"/>
-      <c r="AW7" s="97" t="s">
+      <c r="AQ7" s="95"/>
+      <c r="AR7" s="95"/>
+      <c r="AS7" s="95"/>
+      <c r="AT7" s="95"/>
+      <c r="AU7" s="95"/>
+      <c r="AV7" s="96"/>
+      <c r="AW7" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="AX7" s="97"/>
-      <c r="AY7" s="97"/>
-      <c r="AZ7" s="97"/>
-      <c r="BA7" s="97"/>
-      <c r="BB7" s="97"/>
-      <c r="BC7" s="98"/>
-      <c r="BD7" s="99" t="s">
+      <c r="AX7" s="95"/>
+      <c r="AY7" s="95"/>
+      <c r="AZ7" s="95"/>
+      <c r="BA7" s="95"/>
+      <c r="BB7" s="95"/>
+      <c r="BC7" s="96"/>
+      <c r="BD7" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="BE7" s="97"/>
-      <c r="BF7" s="97"/>
-      <c r="BG7" s="97"/>
-      <c r="BH7" s="97"/>
-      <c r="BI7" s="97"/>
-      <c r="BJ7" s="100"/>
+      <c r="BE7" s="95"/>
+      <c r="BF7" s="95"/>
+      <c r="BG7" s="95"/>
+      <c r="BH7" s="95"/>
+      <c r="BI7" s="95"/>
+      <c r="BJ7" s="98"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2988,7 +2981,9 @@
       <c r="H12" s="60"/>
       <c r="I12" s="61"/>
       <c r="J12" s="61"/>
-      <c r="K12" s="63"/>
+      <c r="K12" s="63">
+        <v>1</v>
+      </c>
       <c r="L12" s="57"/>
       <c r="M12" s="58"/>
       <c r="N12" s="59"/>
@@ -3001,7 +2996,9 @@
       <c r="U12" s="59"/>
       <c r="V12" s="60"/>
       <c r="W12" s="61"/>
-      <c r="X12" s="61"/>
+      <c r="X12" s="61">
+        <v>1</v>
+      </c>
       <c r="Y12" s="63"/>
       <c r="Z12" s="57"/>
       <c r="AA12" s="58"/>
@@ -3426,7 +3423,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3572,7 +3569,7 @@
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="51"/>
@@ -3602,8 +3599,12 @@
       <c r="T20" s="58"/>
       <c r="U20" s="59"/>
       <c r="V20" s="60"/>
-      <c r="W20" s="68"/>
-      <c r="X20" s="68"/>
+      <c r="W20" s="68">
+        <v>0</v>
+      </c>
+      <c r="X20" s="68">
+        <v>3</v>
+      </c>
       <c r="Y20" s="68"/>
       <c r="Z20" s="57"/>
       <c r="AA20" s="58"/>
@@ -3654,7 +3655,7 @@
       </c>
       <c r="D21" s="83">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21" s="50"/>
       <c r="F21" s="52"/>
@@ -3663,7 +3664,7 @@
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
       <c r="K21" s="63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L21" s="57"/>
       <c r="M21" s="58"/>
@@ -3729,7 +3730,7 @@
       </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E22" s="50"/>
       <c r="F22" s="51"/>
@@ -3754,7 +3755,9 @@
       <c r="U22" s="59"/>
       <c r="V22" s="60"/>
       <c r="W22" s="55"/>
-      <c r="X22" s="55"/>
+      <c r="X22" s="55">
+        <v>4</v>
+      </c>
       <c r="Y22" s="56"/>
       <c r="Z22" s="57"/>
       <c r="AA22" s="58"/>
@@ -3823,12 +3826,16 @@
       <c r="Q23" s="5">
         <v>1</v>
       </c>
-      <c r="R23" s="90"/>
+      <c r="R23" s="90">
+        <v>0</v>
+      </c>
       <c r="S23" s="57"/>
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
-      <c r="W23" s="56"/>
+      <c r="W23" s="56" t="s">
+        <v>61</v>
+      </c>
       <c r="Y23" s="56"/>
       <c r="Z23" s="57"/>
       <c r="AA23" s="58"/>
@@ -3897,7 +3904,9 @@
       <c r="Q24" s="55">
         <v>1</v>
       </c>
-      <c r="R24" s="90"/>
+      <c r="R24" s="90">
+        <v>0</v>
+      </c>
       <c r="S24" s="57"/>
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
@@ -3971,7 +3980,9 @@
       <c r="Q25" s="55">
         <v>1</v>
       </c>
-      <c r="R25" s="93"/>
+      <c r="R25" s="103">
+        <v>0</v>
+      </c>
       <c r="S25" s="57"/>
       <c r="T25" s="58"/>
       <c r="U25" s="59"/>
@@ -4045,9 +4056,11 @@
       <c r="T26" s="58"/>
       <c r="U26" s="59"/>
       <c r="V26" s="60"/>
-      <c r="W26" s="94"/>
+      <c r="W26" s="103">
+        <v>0</v>
+      </c>
       <c r="X26" s="90"/>
-      <c r="Y26" s="95"/>
+      <c r="Y26" s="93"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
       <c r="AB26" s="59"/>
@@ -4118,7 +4131,9 @@
       <c r="T27" s="58"/>
       <c r="U27" s="59"/>
       <c r="V27" s="60"/>
-      <c r="W27" s="68"/>
+      <c r="W27" s="68">
+        <v>0</v>
+      </c>
       <c r="X27" s="90"/>
       <c r="Z27" s="57"/>
       <c r="AA27" s="58"/>
@@ -5253,7 +5268,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>38.5</v>
+        <v>44.5</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5327,7 +5342,7 @@
       </c>
       <c r="X43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y43" s="39">
         <f t="shared" si="3"/>
@@ -5528,10 +5543,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.4" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="104"/>
+      <c r="B2" s="102"/>
       <c r="C2" s="79" t="s">
         <v>14</v>
       </c>
@@ -5540,11 +5555,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="101" t="str">
+      <c r="A3" s="99" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="102"/>
+      <c r="B3" s="100"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
         <v>6</v>
@@ -5557,11 +5572,11 @@
       <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="101" t="str">
+      <c r="A4" s="99" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="102"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
         <v>1.5</v>
@@ -5574,28 +5589,28 @@
       <c r="F4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="101" t="str">
+      <c r="A5" s="99" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="102"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
         <v>68</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="101" t="str">
+      <c r="A6" s="99" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="102"/>
+      <c r="B6" s="100"/>
       <c r="C6" s="80">
         <f>Zeitplanung!C31</f>
         <v>1</v>
@@ -5607,11 +5622,11 @@
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="101" t="str">
+      <c r="A7" s="99" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="102"/>
+      <c r="B7" s="100"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
         <v>1</v>
@@ -5623,11 +5638,11 @@
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="101" t="str">
+      <c r="A8" s="99" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="102"/>
+      <c r="B8" s="100"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
         <v>3</v>

</xml_diff>

<commit_message>
An Game Over mit Score Anzeige gearbeitet.
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BLJ\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F32894-7207-4A1C-A7BB-A8EE5511C3A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093CF7A8-09FC-4AA5-AB2D-BED3BC6A3A3A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="4050" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1655,7 +1655,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.5</c:v>
+                  <c:v>51.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2162,8 +2162,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="96" zoomScaleNormal="96" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AG25" sqref="AG25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="96" zoomScaleNormal="96" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AY27" sqref="AY27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3425,7 +3425,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>43.5</v>
+        <v>51.5</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -4044,7 +4044,7 @@
       </c>
       <c r="D26" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E26" s="50"/>
       <c r="F26" s="51"/>
@@ -4087,7 +4087,9 @@
       <c r="AO26" s="58"/>
       <c r="AP26" s="59"/>
       <c r="AQ26" s="60"/>
-      <c r="AR26" s="55"/>
+      <c r="AR26" s="55">
+        <v>8</v>
+      </c>
       <c r="AS26" s="55"/>
       <c r="AT26" s="56"/>
       <c r="AU26" s="57"/>
@@ -5276,7 +5278,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5430,7 +5432,7 @@
       </c>
       <c r="AR43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AS43" s="39">
         <f t="shared" si="4"/>
@@ -5608,7 +5610,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>43.5</v>
+        <v>51.5</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>